<commit_message>
cov sensitivity + FINAL run
got beta in a good spot. model makes sense and is estiamting alpha right.
</commit_message>
<xml_diff>
--- a/writing/Manuscript_Tables_V2.xlsx
+++ b/writing/Manuscript_Tables_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D275D4F1-28C5-E140-B4C3-7AD4D96035B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{574EAAA1-AB28-9744-859E-EF5C7F6851BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8400" yWindow="760" windowWidth="27780" windowHeight="21580" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
+    <workbookView xWindow="11060" yWindow="940" windowWidth="26240" windowHeight="19160" activeTab="3" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Covariates" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="123">
   <si>
     <t>Covariate</t>
   </si>
@@ -277,9 +277,6 @@
     <t>Alaska Climate Research Center</t>
   </si>
   <si>
-    <t>Raymond-Yakoubian J 2009, Jallen et al 2022</t>
-  </si>
-  <si>
     <t>Snow Depth</t>
   </si>
   <si>
@@ -352,60 +349,12 @@
     <t>Monthly Mean Snow Depth (in), summed October - December, 2002-2021</t>
   </si>
   <si>
-    <t>[0.13, 0.99]</t>
-  </si>
-  <si>
-    <t>[0.02, 0.97]</t>
-  </si>
-  <si>
-    <t>[-0.24, 0.15]</t>
-  </si>
-  <si>
-    <t>[-5.92, -5.29]</t>
-  </si>
-  <si>
-    <t>[0.01, 0.06], [0.43,0.99], [0.01, 0.04], [0.13, 0.29]</t>
-  </si>
-  <si>
-    <t>0.03,                   0.81,                        0.28,                   0.02</t>
-  </si>
-  <si>
-    <t>[0.13, 0.39]</t>
-  </si>
-  <si>
-    <t>[0.03, 0.35]</t>
-  </si>
-  <si>
-    <t>[-0.31, -0.02]</t>
-  </si>
-  <si>
-    <t>[-0.30, 0.01]</t>
-  </si>
-  <si>
-    <t>[-0.11, 0.13]</t>
-  </si>
-  <si>
-    <t>[-0.09, 0.15]</t>
-  </si>
-  <si>
-    <t>[0.02, 0.24]</t>
-  </si>
-  <si>
-    <t>[-0.04, 0.15]</t>
-  </si>
-  <si>
     <t>Log carrying capacity for egg to juvenile stage</t>
   </si>
   <si>
     <t>Log carrying capacity for juvenile to marine stage</t>
   </si>
   <si>
-    <t>[15.9,19.9]</t>
-  </si>
-  <si>
-    <t>[15.2,20.4]</t>
-  </si>
-  <si>
     <t>~Normal(16,2)</t>
   </si>
   <si>
@@ -440,6 +389,66 @@
   </si>
   <si>
     <t>Ny,s=r,a</t>
+  </si>
+  <si>
+    <t>0.05,                   0.59,                        0.31,                   0.04</t>
+  </si>
+  <si>
+    <t>[-0.26, 0.13]</t>
+  </si>
+  <si>
+    <t>[-0.05, 0.30]</t>
+  </si>
+  <si>
+    <t>[-0.2, 0.15]</t>
+  </si>
+  <si>
+    <t>[-0.13, 0.23]</t>
+  </si>
+  <si>
+    <t>[0.26, 0.54]</t>
+  </si>
+  <si>
+    <t>[-0.69, -0.37]</t>
+  </si>
+  <si>
+    <t>[-0.55, -0.27]</t>
+  </si>
+  <si>
+    <t>[-0.41, -0.07]</t>
+  </si>
+  <si>
+    <t>[-5.94, -5.73]</t>
+  </si>
+  <si>
+    <t>[0.27, 0.47]</t>
+  </si>
+  <si>
+    <t>[16.28, 19.42]</t>
+  </si>
+  <si>
+    <t>[16.86, 21.81]</t>
+  </si>
+  <si>
+    <t>[0.03, 0.08],
+[0.51, 0.67],
+[0.25, 0.39],
+[0.02, 0.07]</t>
+  </si>
+  <si>
+    <t>4.07,                   5.92,                        6.57,                   7.07</t>
+  </si>
+  <si>
+    <t>[3.67, 4.44], [5.60, 6.19], [6.25, 6.88], [6.72, 7.43]</t>
+  </si>
+  <si>
+    <t>Raymond-Yakoubian 2009, Jallen et al 2022</t>
+  </si>
+  <si>
+    <t>[0.39, 0.44]</t>
+  </si>
+  <si>
+    <t>[0.01, 0.1]</t>
   </si>
 </sst>
 </file>
@@ -515,7 +524,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -909,12 +918,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1115,19 +1137,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1143,12 +1152,48 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2277,8 +2322,8 @@
       <xdr:rowOff>19967</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="183575" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -2320,6 +2365,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2362,7 +2408,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -5637,8 +5683,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="183575" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -5680,6 +5726,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5722,7 +5769,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -5799,8 +5846,8 @@
       <xdr:rowOff>9588</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="270523" cy="176651"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -5842,6 +5889,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -5898,7 +5946,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="TextBox 1">
@@ -6284,8 +6332,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C922C39-C49D-8D4D-BCBE-7247337ED328}">
   <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="90" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6293,9 +6341,10 @@
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="40.83203125" style="1" customWidth="1"/>
-    <col min="4" max="5" width="32.83203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="1"/>
-    <col min="7" max="7" width="20.5" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.83203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.33203125" style="1" customWidth="1"/>
     <col min="8" max="8" width="24" style="1" customWidth="1"/>
     <col min="9" max="9" width="32.83203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" style="1" customWidth="1"/>
@@ -6336,7 +6385,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E2" s="45">
         <v>0</v>
@@ -6360,10 +6409,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E3" s="44">
         <v>0</v>
@@ -6372,10 +6421,10 @@
         <v>4</v>
       </c>
       <c r="G3" s="58" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>66</v>
+        <v>120</v>
       </c>
       <c r="I3" s="40" t="s">
         <v>65</v>
@@ -6390,7 +6439,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E4" s="55">
         <v>1</v>
@@ -6416,7 +6465,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E5" s="45">
         <v>1</v>
@@ -6442,7 +6491,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E6" s="43">
         <v>2</v>
@@ -6468,7 +6517,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E7" s="44">
         <v>2</v>
@@ -6494,7 +6543,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E8" s="46">
         <v>2</v>
@@ -6512,15 +6561,21 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
-      <c r="C13" s="5" t="s">
+    <row r="10" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="C10" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="85" x14ac:dyDescent="0.2">
-      <c r="C14" s="4" t="s">
+    <row r="11" spans="1:10" ht="85" x14ac:dyDescent="0.2">
+      <c r="C11" s="4" t="s">
         <v>54</v>
       </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6531,8 +6586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F6D1E8C-B800-DB41-95B4-3695A974BBA7}">
   <dimension ref="B1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="173" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:D9"/>
+    <sheetView zoomScale="137" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6620,11 +6675,11 @@
     </row>
     <row r="9" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B9" s="37"/>
-      <c r="C9" s="87" t="s">
-        <v>114</v>
+      <c r="C9" s="82" t="s">
+        <v>97</v>
       </c>
       <c r="D9" s="76" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="17" x14ac:dyDescent="0.2">
@@ -6654,7 +6709,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6673,10 +6728,10 @@
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
@@ -6760,23 +6815,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8EA89-DADA-994F-B9EB-DFFAA747018D}">
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScale="106" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="81" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="32" customWidth="1"/>
-    <col min="3" max="3" width="15" style="84" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="85" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" style="31" customWidth="1"/>
+    <col min="3" max="3" width="15" style="79" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="61" customWidth="1"/>
-    <col min="5" max="5" width="22.33203125" customWidth="1"/>
-    <col min="7" max="7" width="2.5" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="88" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="88"/>
+    <col min="7" max="7" width="2.5" style="88" customWidth="1"/>
+    <col min="8" max="8" width="19.6640625" style="88" customWidth="1"/>
+    <col min="9" max="16384" width="10.83203125" style="88"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="84" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="85" t="s">
+    <row r="1" spans="1:8" s="79" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A1" s="80" t="s">
         <v>64</v>
       </c>
       <c r="B1" s="22" t="s">
@@ -6788,263 +6845,267 @@
       <c r="D1" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="E1" s="86" t="s">
+      <c r="E1" s="81" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="75"/>
-      <c r="B2" s="77" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="82">
-        <v>0.7</v>
+      <c r="B2" s="86" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="96">
+        <v>0.05</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="E2" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="E2" s="87" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="75"/>
-      <c r="B3" s="77" t="s">
-        <v>81</v>
-      </c>
-      <c r="C3" s="82">
-        <v>0.51</v>
+      <c r="B3" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" s="77">
+        <v>0.42</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>92</v>
-      </c>
-      <c r="E3" s="36" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="87" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="75"/>
-      <c r="B4" s="77" t="s">
+      <c r="B4" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C4" s="82">
-        <v>0.17</v>
+      <c r="C4" s="77">
+        <v>-0.06</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="E4" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="E4" s="87" t="s">
         <v>37</v>
       </c>
       <c r="H4" s="61"/>
     </row>
     <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A5" s="75"/>
-      <c r="B5" s="77" t="s">
+      <c r="B5" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="82">
-        <v>0.09</v>
+      <c r="C5" s="77">
+        <v>0.12</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5" s="36" t="s">
+        <v>106</v>
+      </c>
+      <c r="E5" s="87" t="s">
         <v>37</v>
       </c>
       <c r="H5" s="61"/>
     </row>
     <row r="6" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="75"/>
-      <c r="B6" s="77" t="s">
+      <c r="B6" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="82">
-        <v>0.02</v>
+      <c r="C6" s="77">
+        <v>-0.02</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>101</v>
-      </c>
-      <c r="E6" s="36" t="s">
+        <v>107</v>
+      </c>
+      <c r="E6" s="87" t="s">
         <v>37</v>
       </c>
       <c r="H6" s="61"/>
     </row>
     <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A7" s="75"/>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C7" s="82">
-        <v>0.01</v>
+      <c r="C7" s="77">
+        <v>0.06</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="E7" s="36" t="s">
+        <v>108</v>
+      </c>
+      <c r="E7" s="87" t="s">
         <v>37</v>
       </c>
       <c r="H7" s="61"/>
     </row>
     <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="75"/>
-      <c r="B8" s="77" t="s">
+      <c r="B8" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="82">
-        <v>0.16</v>
+      <c r="C8" s="77">
+        <v>0.4</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="E8" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="E8" s="87" t="s">
         <v>37</v>
       </c>
       <c r="H8" s="61"/>
     </row>
     <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A9" s="75"/>
-      <c r="B9" s="77" t="s">
+      <c r="B9" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C9" s="82">
-        <v>-0.13</v>
+      <c r="C9" s="77">
+        <v>-0.53</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="E9" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E9" s="87" t="s">
         <v>37</v>
       </c>
       <c r="H9" s="61"/>
     </row>
     <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A10" s="75"/>
-      <c r="B10" s="77" t="s">
+      <c r="B10" s="86" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="82">
-        <v>-0.12</v>
+      <c r="C10" s="77">
+        <v>-0.4</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="E10" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E10" s="87" t="s">
         <v>37</v>
       </c>
       <c r="H10" s="61"/>
     </row>
-    <row r="11" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="90"/>
-      <c r="B11" s="89" t="s">
-        <v>116</v>
-      </c>
-      <c r="C11" s="88"/>
-      <c r="D11" s="24"/>
+    <row r="11" spans="1:8" ht="68" x14ac:dyDescent="0.2">
+      <c r="A11" s="89"/>
+      <c r="B11" s="90" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="83" t="s">
+        <v>118</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>119</v>
+      </c>
       <c r="E11" s="91" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="H11" s="61"/>
     </row>
     <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="75"/>
-      <c r="B12" s="77" t="s">
+      <c r="B12" s="86" t="s">
         <v>39</v>
       </c>
-      <c r="C12" s="82">
-        <v>-0.04</v>
-      </c>
-      <c r="D12" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="E12" s="36" t="s">
+      <c r="C12" s="77">
+        <v>-0.24</v>
+      </c>
+      <c r="D12" s="92" t="s">
+        <v>112</v>
+      </c>
+      <c r="E12" s="87" t="s">
         <v>34</v>
       </c>
       <c r="H12" s="61"/>
     </row>
     <row r="13" spans="1:8" ht="73" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="75"/>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="82">
-        <v>-5.61</v>
-      </c>
-      <c r="D13" s="24" t="s">
-        <v>94</v>
-      </c>
-      <c r="E13" s="36" t="s">
+      <c r="C13" s="77">
+        <v>-5.83</v>
+      </c>
+      <c r="D13" s="92" t="s">
+        <v>113</v>
+      </c>
+      <c r="E13" s="87" t="s">
         <v>46</v>
       </c>
       <c r="H13" s="61"/>
     </row>
     <row r="14" spans="1:8" ht="68" x14ac:dyDescent="0.2">
       <c r="A14" s="75"/>
-      <c r="B14" s="77" t="s">
-        <v>111</v>
+      <c r="B14" s="86" t="s">
+        <v>94</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="D14" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="E14" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="E14" s="87" t="s">
         <v>35</v>
       </c>
       <c r="H14" s="61"/>
     </row>
     <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="75"/>
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="86" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="82">
-        <v>0.21</v>
-      </c>
-      <c r="D15" s="24" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" s="36" t="s">
+      <c r="C15" s="77">
+        <v>0.36</v>
+      </c>
+      <c r="D15" s="92" t="s">
+        <v>114</v>
+      </c>
+      <c r="E15" s="87" t="s">
         <v>35</v>
       </c>
       <c r="H15" s="61"/>
     </row>
     <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="79"/>
-      <c r="B16" s="77" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" s="82">
-        <v>17.27</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>108</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>109</v>
+      <c r="A16" s="93"/>
+      <c r="B16" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="77">
+        <v>17.28</v>
+      </c>
+      <c r="D16" s="92" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="87" t="s">
+        <v>92</v>
       </c>
       <c r="H16" s="61"/>
     </row>
     <row r="17" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="80"/>
-      <c r="B17" s="78" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="83">
-        <v>17.57</v>
-      </c>
-      <c r="D17" s="27" t="s">
-        <v>107</v>
-      </c>
-      <c r="E17" s="76" t="s">
-        <v>110</v>
+      <c r="A17" s="84"/>
+      <c r="B17" s="63" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" s="78">
+        <v>18.96</v>
+      </c>
+      <c r="D17" s="94" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="95" t="s">
+        <v>93</v>
       </c>
       <c r="H17" s="61"/>
     </row>
     <row r="21" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="B21" s="32" t="s">
-        <v>68</v>
+      <c r="B21" s="31" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -7070,13 +7131,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="65" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="65" t="s">
-        <v>71</v>
-      </c>
       <c r="C1" s="72" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D1" s="66" t="s">
         <v>1</v>
@@ -7084,80 +7145,80 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="67" t="s">
-        <v>117</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C2" s="73">
         <v>4.1100000000000003</v>
       </c>
       <c r="D2" s="68" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="67"/>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" s="73">
         <v>4.12</v>
       </c>
       <c r="D3" s="68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="67" t="s">
-        <v>120</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="73">
         <v>4.13</v>
       </c>
       <c r="D4" s="68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="67" t="s">
-        <v>118</v>
+        <v>101</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C5" s="73">
         <v>4.1399999999999997</v>
       </c>
       <c r="D5" s="68" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="69" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B6" s="70" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C6" s="74">
         <v>4.1500000000000004</v>
       </c>
       <c r="D6" s="71" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start responses to internal review
</commit_message>
<xml_diff>
--- a/writing/Manuscript_Tables_V2.xlsx
+++ b/writing/Manuscript_Tables_V2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/genoasullaway/Documents/GitHub/AYK_prey/writing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24FA28EE-1311-C842-B2B3-D454D1782163}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C6C88F0-DB03-2547-9A96-9E24B918BD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="34560" yWindow="500" windowWidth="37460" windowHeight="21100" activeTab="1" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
+    <workbookView xWindow="4520" yWindow="760" windowWidth="30040" windowHeight="20560" activeTab="1" xr2:uid="{15635B22-154F-5C4D-8D09-E55D0FC35932}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1 Covariates" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="121">
   <si>
     <t>Covariate</t>
   </si>
@@ -168,9 +168,6 @@
     <t xml:space="preserve">Log-normal mean instantaneous fishing mortality </t>
   </si>
   <si>
-    <t xml:space="preserve">Covariate coefficient for juvenile and marine covariates </t>
-  </si>
-  <si>
     <t>Brood Year Offset</t>
   </si>
   <si>
@@ -186,9 +183,6 @@
     <t>Model Stage Implemented</t>
   </si>
   <si>
-    <t>~Normal(-5,1)</t>
-  </si>
-  <si>
     <t>Link</t>
   </si>
   <si>
@@ -279,12 +273,6 @@
     <t xml:space="preserve">Data sources and related equations in the text. </t>
   </si>
   <si>
-    <t>Basal productivity for marine stage</t>
-  </si>
-  <si>
-    <t>Basal productivity for juvenile stage</t>
-  </si>
-  <si>
     <t xml:space="preserve">Insulating properties of snow enhances egg productivity during cold winters  </t>
   </si>
   <si>
@@ -354,28 +342,7 @@
     <t>[-0.26, 0.13]</t>
   </si>
   <si>
-    <t>[-0.05, 0.30]</t>
-  </si>
-  <si>
-    <t>[-0.2, 0.15]</t>
-  </si>
-  <si>
-    <t>[-0.13, 0.23]</t>
-  </si>
-  <si>
     <t>[0.26, 0.54]</t>
-  </si>
-  <si>
-    <t>[-0.69, -0.37]</t>
-  </si>
-  <si>
-    <t>[-0.55, -0.27]</t>
-  </si>
-  <si>
-    <t>[-0.41, -0.07]</t>
-  </si>
-  <si>
-    <t>[-5.94, -5.73]</t>
   </si>
   <si>
     <t>[0.27, 0.47]</t>
@@ -393,29 +360,77 @@
 [0.02, 0.07]</t>
   </si>
   <si>
-    <t>4.07,                   5.92,                        6.57,                   7.07</t>
-  </si>
-  <si>
-    <t>[3.67, 4.44], [5.60, 6.19], [6.25, 6.88], [6.72, 7.43]</t>
-  </si>
-  <si>
     <t>Raymond-Yakoubian 2009, Jallen et al 2022</t>
   </si>
   <si>
-    <t>[0.12, 0.89]</t>
-  </si>
-  <si>
-    <t>[0.02, 0.33]</t>
-  </si>
-  <si>
     <t>~Beta(0,1.5)</t>
+  </si>
+  <si>
+    <t>Logit basal productivity for juvenile stage</t>
+  </si>
+  <si>
+    <t>Logit basal productivity for marine stage</t>
+  </si>
+  <si>
+    <t>[-2.48,0.20]</t>
+  </si>
+  <si>
+    <t>[-2.95,-1.08]</t>
+  </si>
+  <si>
+    <t>[0.11, 0.41]</t>
+  </si>
+  <si>
+    <t>[-0.05, 0.27]</t>
+  </si>
+  <si>
+    <t>[-0.23, 0.08]</t>
+  </si>
+  <si>
+    <t>[-0.44, -0.21]</t>
+  </si>
+  <si>
+    <t>[-0.31, -0.08]</t>
+  </si>
+  <si>
+    <t>3.87,                   5.92,                        4.57,                   8.04</t>
+  </si>
+  <si>
+    <t>[1.18, 6.44], [4.60, 7.19], [3.25, 6.88], [6.72, 9.50]</t>
+  </si>
+  <si>
+    <t>[-4.08, -0.12]</t>
+  </si>
+  <si>
+    <t>~Normal(0,5)</t>
+  </si>
+  <si>
+    <t>[-8.94, -6.63]</t>
+  </si>
+  <si>
+    <t>Covariate Parameters and Estimate</t>
+  </si>
+  <si>
+    <t>Population Dynamics Parameters and Estimates</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>Juvenile</t>
+  </si>
+  <si>
+    <t>Escapement</t>
+  </si>
+  <si>
+    <t>Covariate coefficient</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -475,6 +490,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -484,7 +513,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="32">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -891,12 +920,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1116,17 +1184,59 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1150,14 +1260,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>17956</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>11385</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="292259" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -1199,7 +1309,6 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a14:m>
                 <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:r>
@@ -1236,7 +1345,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="TextBox 6">
@@ -1306,9 +1415,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>4816</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>3</xdr:row>
       <xdr:rowOff>7007</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="333553" cy="173702"/>
@@ -1479,14 +1588,14 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>11503</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>12786</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="298736" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -1528,7 +1637,6 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
-              <a:pPr/>
               <a14:m>
                 <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:r>
@@ -1562,7 +1670,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="TextBox 10">
@@ -1624,9 +1732,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>31823</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>8829</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="182614" cy="173702"/>
@@ -1780,9 +1888,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>43794</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>8</xdr:row>
       <xdr:rowOff>17224</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="128112" cy="173702"/>
@@ -1909,20 +2017,20 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>215900</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4816</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7007</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="610936" cy="176651"/>
+    <xdr:ext cx="287386" cy="182871"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="TextBox 13">
+            <xdr:cNvPr id="23" name="TextBox 22">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEB54CD-AAA9-5343-ABB4-63631744A2A4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF29C7BF-FC74-754D-8780-016FB362B2CD}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1930,7 +2038,778 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="2802363"/>
+              <a:off x="4816" y="2160927"/>
+              <a:ext cx="287386" cy="182871"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝛽</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑠</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>=</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑗</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="23" name="TextBox 22">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF29C7BF-FC74-754D-8780-016FB362B2CD}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="4816" y="2160927"/>
+              <a:ext cx="287386" cy="182871"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝛽_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠=𝑗)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2997</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="852606" cy="182871"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E756816A-9971-73D1-3630-2F3EF17BEB92}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="9778502"/>
+              <a:ext cx="852606" cy="182871"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:r>
+                    <m:rPr>
+                      <m:sty m:val="p"/>
+                    </m:rPr>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>ln</m:t>
+                  </m:r>
+                  <m:r>
+                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                    </a:rPr>
+                    <m:t>⁡(</m:t>
+                  </m:r>
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝜂</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑠</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>=</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑗𝑢𝑣𝑒𝑛𝑖𝑙𝑒</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>)</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="3" name="TextBox 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E756816A-9971-73D1-3630-2F3EF17BEB92}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="0" y="9778502"/>
+              <a:ext cx="852606" cy="182871"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>ln⁡(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜂_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠=𝑗𝑢𝑣𝑒𝑛𝑖𝑙𝑒)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>)</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>6136</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>23400</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="802143" cy="173702"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B0D1554-1690-444C-B763-15D3975AA76D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6136" y="10230006"/>
+              <a:ext cx="802143" cy="173702"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:sSub>
+                    <m:sSubPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:sSubPr>
+                    <m:e>
+                      <m:r>
+                        <m:rPr>
+                          <m:sty m:val="p"/>
+                        </m:rPr>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>ln</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>⁡(</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝜂</m:t>
+                      </m:r>
+                    </m:e>
+                    <m:sub>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑠</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>=</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>𝑚𝑎𝑟𝑖𝑛𝑒</m:t>
+                      </m:r>
+                    </m:sub>
+                  </m:sSub>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>)</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="4" name="TextBox 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B0D1554-1690-444C-B763-15D3975AA76D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6136" y="10230006"/>
+              <a:ext cx="802143" cy="173702"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>ln⁡(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝜂〗_(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑠=𝑚𝑎𝑟𝑖𝑛𝑒)</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100"/>
+                <a:t>)</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>14940</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="417678" cy="173702"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0C7D6A6-31BC-7242-BD4A-702ECF46289B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="829235" y="1516528"/>
+              <a:ext cx="417678" cy="173702"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:sSub>
+                      <m:sSubPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:sSubPr>
+                      <m:e>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>ln</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>⁡(</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝛼</m:t>
+                        </m:r>
+                      </m:e>
+                      <m:sub>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑎</m:t>
+                        </m:r>
+                      </m:sub>
+                    </m:sSub>
+                    <m:r>
+                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                      </a:rPr>
+                      <m:t>)</m:t>
+                    </m:r>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback xmlns="">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0C7D6A6-31BC-7242-BD4A-702ECF46289B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="829235" y="1516528"/>
+              <a:ext cx="417678" cy="173702"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr/>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>〖</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>ln⁡(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝛼〗_</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>𝑎)</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>22412</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>21665</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="610936" cy="176651"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="25" name="TextBox 24">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82781835-9E85-DF4B-A452-A11A65848FA0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="851647" y="6565900"/>
               <a:ext cx="610936" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2079,13 +2958,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="14" name="TextBox 13">
+            <xdr:cNvPr id="25" name="TextBox 24">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8CEB54CD-AAA9-5343-ABB4-63631744A2A4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{82781835-9E85-DF4B-A452-A11A65848FA0}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2093,7 +2972,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="2802363"/>
+              <a:off x="851647" y="6565900"/>
               <a:ext cx="610936" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2156,20 +3035,20 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>14941</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>14941</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1125244" cy="176651"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="TextBox 5">
+            <xdr:cNvPr id="26" name="TextBox 25">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28901B06-A5F3-0343-9499-5F1CED09E050}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB2F798-4B39-684F-9D47-261DF441E29A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2177,7 +3056,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="3236951"/>
+              <a:off x="844176" y="6775823"/>
               <a:ext cx="1125244" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2371,13 +3250,13 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="6" name="TextBox 5">
+            <xdr:cNvPr id="26" name="TextBox 25">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{28901B06-A5F3-0343-9499-5F1CED09E050}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CB2F798-4B39-684F-9D47-261DF441E29A}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2385,7 +3264,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="3236951"/>
+              <a:off x="844176" y="6775823"/>
               <a:ext cx="1125244" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2472,9 +3351,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1596912" cy="176651"/>
@@ -2482,10 +3361,10 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="TextBox 15">
+            <xdr:cNvPr id="27" name="TextBox 26">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E786A63-156D-3849-A1B6-1234AF094683}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ACE4C99-D3CF-2A46-9425-1C0981A3B24C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2493,7 +3372,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="3422805"/>
+              <a:off x="829235" y="2368176"/>
               <a:ext cx="1596912" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2675,10 +3554,10 @@
       <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="16" name="TextBox 15">
+            <xdr:cNvPr id="27" name="TextBox 26">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E786A63-156D-3849-A1B6-1234AF094683}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8ACE4C99-D3CF-2A46-9425-1C0981A3B24C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2686,7 +3565,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="3422805"/>
+              <a:off x="829235" y="2368176"/>
               <a:ext cx="1596912" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2749,9 +3628,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>8301</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="918136" cy="176651"/>
@@ -2759,10 +3638,10 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="17" name="TextBox 16">
+            <xdr:cNvPr id="28" name="TextBox 27">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E1C9E8F-ACF9-7F44-9A2F-6E6AA5F94A83}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F439FC95-0BD5-0A41-A9E1-0B79414A6B42}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2770,7 +3649,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4427901"/>
+              <a:off x="829235" y="2989066"/>
               <a:ext cx="918136" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2952,10 +3831,10 @@
       <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="17" name="TextBox 16">
+            <xdr:cNvPr id="28" name="TextBox 27">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E1C9E8F-ACF9-7F44-9A2F-6E6AA5F94A83}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F439FC95-0BD5-0A41-A9E1-0B79414A6B42}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -2963,7 +3842,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4427901"/>
+              <a:off x="829235" y="2989066"/>
               <a:ext cx="918136" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3026,9 +3905,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1269578" cy="176651"/>
@@ -3036,10 +3915,10 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18" name="TextBox 17">
+            <xdr:cNvPr id="29" name="TextBox 28">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCB90B6E-049C-5841-BB92-4A602A652C76}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A95D745D-0C0C-5F4F-A349-F35BB312AF63}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3047,7 +3926,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4622800"/>
+              <a:off x="829235" y="3414059"/>
               <a:ext cx="1269578" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3244,10 +4123,10 @@
       <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="18" name="TextBox 17">
+            <xdr:cNvPr id="29" name="TextBox 28">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FCB90B6E-049C-5841-BB92-4A602A652C76}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A95D745D-0C0C-5F4F-A349-F35BB312AF63}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3255,7 +4134,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4622800"/>
+              <a:off x="829235" y="3414059"/>
               <a:ext cx="1269578" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3318,9 +4197,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1173335" cy="176651"/>
@@ -3328,10 +4207,10 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="19" name="TextBox 18">
+            <xdr:cNvPr id="30" name="TextBox 29">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F359704E-DC62-9A41-B15E-32AB5838B462}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BEC71E8-0915-A24D-A869-ECB98547863E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3339,7 +4218,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4826000"/>
+              <a:off x="829235" y="3847353"/>
               <a:ext cx="1173335" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3521,10 +4400,10 @@
       <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="19" name="TextBox 18">
+            <xdr:cNvPr id="30" name="TextBox 29">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F359704E-DC62-9A41-B15E-32AB5838B462}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BEC71E8-0915-A24D-A869-ECB98547863E}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3532,7 +4411,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="4826000"/>
+              <a:off x="829235" y="3847353"/>
               <a:ext cx="1173335" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3595,9 +4474,9 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="1304011" cy="176651"/>
@@ -3605,10 +4484,10 @@
       <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="20" name="TextBox 19">
+            <xdr:cNvPr id="31" name="TextBox 30">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00A12E55-7098-5C49-A7F2-10DC08B956A6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CAABD7F-4DF1-1A4C-BA62-77CD05584C9D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3616,7 +4495,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="5029200"/>
+              <a:off x="829235" y="4280647"/>
               <a:ext cx="1304011" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3798,10 +4677,10 @@
       <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="20" name="TextBox 19">
+            <xdr:cNvPr id="31" name="TextBox 30">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00A12E55-7098-5C49-A7F2-10DC08B956A6}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4CAABD7F-4DF1-1A4C-BA62-77CD05584C9D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -3809,7 +4688,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="0" y="5029200"/>
+              <a:off x="829235" y="4280647"/>
               <a:ext cx="1304011" cy="176651"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -3863,779 +4742,6 @@
                 <a:t> "= Chum Hatchery"</a:t>
               </a:r>
               <a:endParaRPr lang="en-US" sz="1100" i="0"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4816</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>7007</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="287386" cy="182871"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="23" name="TextBox 22">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF29C7BF-FC74-754D-8780-016FB362B2CD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4816" y="2160927"/>
-              <a:ext cx="287386" cy="182871"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝛽</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑠</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>=</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑗</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="23" name="TextBox 22">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF29C7BF-FC74-754D-8780-016FB362B2CD}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="4816" y="2160927"/>
-              <a:ext cx="287386" cy="182871"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝛽_(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑠=𝑗)</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>2997</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="852606" cy="182871"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E756816A-9971-73D1-3630-2F3EF17BEB92}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="9778502"/>
-              <a:ext cx="852606" cy="182871"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:r>
-                    <m:rPr>
-                      <m:sty m:val="p"/>
-                    </m:rPr>
-                    <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>ln</m:t>
-                  </m:r>
-                  <m:r>
-                    <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                      <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                    </a:rPr>
-                    <m:t>⁡(</m:t>
-                  </m:r>
-                  <m:sSub>
-                    <m:sSubPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-US" sz="1100" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝜂</m:t>
-                      </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑠</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>=</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑗𝑢𝑣𝑒𝑛𝑖𝑙𝑒</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
-                </m:oMath>
-              </a14:m>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>)</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="3" name="TextBox 2">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E756816A-9971-73D1-3630-2F3EF17BEB92}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="9778502"/>
-              <a:ext cx="852606" cy="182871"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>ln⁡(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝜂_(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑠=𝑗𝑢𝑣𝑒𝑛𝑖𝑙𝑒)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>)</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>6136</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>23400</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="802143" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="TextBox 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B0D1554-1690-444C-B763-15D3975AA76D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6136" y="10230006"/>
-              <a:ext cx="802143" cy="173702"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:sSub>
-                    <m:sSubPr>
-                      <m:ctrlPr>
-                        <a:rPr lang="en-US" sz="1100" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                      </m:ctrlPr>
-                    </m:sSubPr>
-                    <m:e>
-                      <m:r>
-                        <m:rPr>
-                          <m:sty m:val="p"/>
-                        </m:rPr>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>ln</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>⁡(</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝜂</m:t>
-                      </m:r>
-                    </m:e>
-                    <m:sub>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑠</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>=</m:t>
-                      </m:r>
-                      <m:r>
-                        <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        </a:rPr>
-                        <m:t>𝑚𝑎𝑟𝑖𝑛𝑒</m:t>
-                      </m:r>
-                    </m:sub>
-                  </m:sSub>
-                </m:oMath>
-              </a14:m>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>)</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="4" name="TextBox 3">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1B0D1554-1690-444C-B763-15D3975AA76D}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="6136" y="10230006"/>
-              <a:ext cx="802143" cy="173702"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>ln⁡(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝜂〗_(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑠=𝑚𝑎𝑟𝑖𝑛𝑒)</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100"/>
-                <a:t>)</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="417678" cy="173702"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0C7D6A6-31BC-7242-BD4A-702ECF46289B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="5814037"/>
-              <a:ext cx="417678" cy="173702"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <m:rPr>
-                            <m:sty m:val="p"/>
-                          </m:rPr>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>ln</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>⁡(</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝛼</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑎</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                        <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>)</m:t>
-                    </m:r>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="en-US" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="TextBox 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0C7D6A6-31BC-7242-BD4A-702ECF46289B}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="0" y="5814037"/>
-              <a:ext cx="417678" cy="173702"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:spAutoFit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>〖</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>ln⁡(</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝛼〗_</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="en-US" sz="1100" b="0" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑎)</a:t>
-              </a:r>
-              <a:endParaRPr lang="en-US" sz="1100"/>
             </a:p>
           </xdr:txBody>
         </xdr:sp>
@@ -5163,7 +5269,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="18" t="s">
         <v>11</v>
@@ -5172,7 +5278,7 @@
         <v>24</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F1" s="18" t="s">
         <v>2</v>
@@ -5195,7 +5301,7 @@
         <v>8</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E2" s="35">
         <v>0</v>
@@ -5204,7 +5310,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="32" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="24" t="s">
         <v>14</v>
@@ -5219,10 +5325,10 @@
         <v>10</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E3" s="34">
         <v>0</v>
@@ -5231,13 +5337,13 @@
         <v>4</v>
       </c>
       <c r="G3" s="48" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H3" s="23" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="I3" s="30" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="J3" s="49"/>
     </row>
@@ -5249,7 +5355,7 @@
         <v>20</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E4" s="45">
         <v>1</v>
@@ -5258,10 +5364,10 @@
         <v>4</v>
       </c>
       <c r="G4" s="47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" s="51" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I4" s="42" t="s">
         <v>21</v>
@@ -5275,7 +5381,7 @@
         <v>19</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E5" s="35">
         <v>1</v>
@@ -5284,10 +5390,10 @@
         <v>4</v>
       </c>
       <c r="G5" s="24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H5" s="24" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I5" s="29" t="s">
         <v>23</v>
@@ -5301,7 +5407,7 @@
         <v>7</v>
       </c>
       <c r="D6" s="21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E6" s="33">
         <v>2</v>
@@ -5316,7 +5422,7 @@
         <v>26</v>
       </c>
       <c r="I6" s="28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="153" x14ac:dyDescent="0.2">
@@ -5327,7 +5433,7 @@
         <v>6</v>
       </c>
       <c r="D7" s="23" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E7" s="34">
         <v>2</v>
@@ -5353,7 +5459,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E8" s="36">
         <v>2</v>
@@ -5378,7 +5484,7 @@
     </row>
     <row r="11" spans="1:10" ht="85" x14ac:dyDescent="0.2">
       <c r="C11" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -5394,302 +5500,381 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1D8EA89-DADA-994F-B9EB-DFFAA747018D}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="170" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.5" style="72" customWidth="1"/>
-    <col min="2" max="2" width="24.83203125" style="27" customWidth="1"/>
-    <col min="3" max="3" width="22.33203125" style="75" customWidth="1"/>
-    <col min="4" max="4" width="15" style="68" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" style="51" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="75"/>
-    <col min="7" max="7" width="12.5" style="75" customWidth="1"/>
-    <col min="8" max="8" width="19.6640625" style="75" customWidth="1"/>
-    <col min="9" max="16384" width="10.83203125" style="75"/>
+    <col min="1" max="1" width="10.83203125" style="75"/>
+    <col min="2" max="3" width="22.5" style="72" customWidth="1"/>
+    <col min="4" max="4" width="24.83203125" style="27" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="75" customWidth="1"/>
+    <col min="6" max="6" width="15" style="68" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="51" customWidth="1"/>
+    <col min="8" max="8" width="10.83203125" style="75"/>
+    <col min="9" max="9" width="12.5" style="75" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" style="75" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="75"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="68" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A1" s="69" t="s">
-        <v>57</v>
-      </c>
-      <c r="B1" s="21" t="s">
+    <row r="1" spans="1:10" s="68" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="B1" s="69" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="70" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="G1" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="70" t="s">
-        <v>31</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="2" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="65"/>
-      <c r="B2" s="73" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="74" t="s">
+    <row r="2" spans="1:10" s="68" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="90" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="91"/>
+      <c r="C2" s="84"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+    </row>
+    <row r="3" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B3" s="65"/>
+      <c r="C3" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="73" t="s">
+        <v>101</v>
+      </c>
+      <c r="E3" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="F3" s="66">
+        <v>-1.07</v>
+      </c>
+      <c r="G3" s="23" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B4" s="65"/>
+      <c r="C4" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="73" t="s">
+        <v>102</v>
+      </c>
+      <c r="E4" s="74" t="s">
+        <v>100</v>
+      </c>
+      <c r="F4" s="66">
+        <v>-1.93</v>
+      </c>
+      <c r="G4" s="23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="B5" s="76"/>
+      <c r="C5" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="77" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>110</v>
+      </c>
+      <c r="G5" s="23" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5" s="51"/>
+    </row>
+    <row r="6" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="B6" s="65"/>
+      <c r="C6" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="73" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="66">
+        <v>-1.84</v>
+      </c>
+      <c r="G6" s="81" t="s">
+        <v>112</v>
+      </c>
+      <c r="J6" s="51"/>
+    </row>
+    <row r="7" spans="1:10" ht="73" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B7" s="65"/>
+      <c r="C7" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="74" t="s">
+        <v>113</v>
+      </c>
+      <c r="F7" s="66">
+        <v>-7.32</v>
+      </c>
+      <c r="G7" s="81" t="s">
+        <v>114</v>
+      </c>
+      <c r="J7" s="51"/>
+    </row>
+    <row r="8" spans="1:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="B8" s="65"/>
+      <c r="C8" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="D8" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="E8" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="23" t="s">
+        <v>92</v>
+      </c>
+      <c r="G8" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="J8" s="51"/>
+    </row>
+    <row r="9" spans="1:10" ht="51" x14ac:dyDescent="0.2">
+      <c r="B9" s="65"/>
+      <c r="C9" s="95" t="s">
+        <v>119</v>
+      </c>
+      <c r="D9" s="73" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="66">
+        <v>0.36</v>
+      </c>
+      <c r="G9" s="81" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="51"/>
+    </row>
+    <row r="10" spans="1:10" ht="34" x14ac:dyDescent="0.2">
+      <c r="B10" s="79"/>
+      <c r="C10" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="D10" s="73" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="66">
+        <v>17.28</v>
+      </c>
+      <c r="G10" s="81" t="s">
+        <v>96</v>
+      </c>
+      <c r="J10" s="51"/>
+    </row>
+    <row r="11" spans="1:10" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="71"/>
+      <c r="C11" s="96" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="E11" s="80" t="s">
+        <v>82</v>
+      </c>
+      <c r="F11" s="67">
+        <v>18.96</v>
+      </c>
+      <c r="G11" s="82" t="s">
+        <v>97</v>
+      </c>
+      <c r="J11" s="51"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="92" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="66">
-        <v>0.52</v>
-      </c>
-      <c r="E2" s="23" t="s">
-        <v>113</v>
-      </c>
+      <c r="B12" s="93"/>
+      <c r="C12" s="89"/>
+      <c r="D12" s="85"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="87"/>
+      <c r="G12" s="88"/>
+      <c r="J12" s="51"/>
     </row>
-    <row r="3" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="65"/>
-      <c r="B3" s="73" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="74" t="s">
-        <v>115</v>
-      </c>
-      <c r="D3" s="66">
-        <v>0.15</v>
-      </c>
-      <c r="E3" s="23" t="s">
-        <v>114</v>
-      </c>
+    <row r="13" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B13" s="65"/>
+      <c r="C13" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="D13" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="E13" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="F13" s="66">
+        <v>-0.1</v>
+      </c>
+      <c r="G13" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="J13" s="51"/>
     </row>
-    <row r="4" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A4" s="65"/>
-      <c r="B4" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" s="74" t="s">
+    <row r="14" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B14" s="65"/>
+      <c r="C14" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="E14" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D4" s="66">
-        <v>-0.06</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>97</v>
-      </c>
-      <c r="H4" s="51"/>
+      <c r="F14" s="66">
+        <v>0.25</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J14" s="51"/>
     </row>
-    <row r="5" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A5" s="65"/>
-      <c r="B5" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="74" t="s">
+    <row r="15" spans="1:10" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="65"/>
+      <c r="C15" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="D15" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="E15" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D5" s="66">
-        <v>0.12</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="51"/>
+      <c r="F15" s="66">
+        <v>0.11</v>
+      </c>
+      <c r="G15" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="J15" s="51"/>
     </row>
-    <row r="6" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="65"/>
-      <c r="B6" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="C6" s="74" t="s">
+    <row r="16" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B16" s="65"/>
+      <c r="C16" s="95" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="E16" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D6" s="66">
-        <v>-0.02</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="H6" s="51"/>
+      <c r="F16" s="66">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>107</v>
+      </c>
+      <c r="J16" s="51"/>
     </row>
-    <row r="7" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="65"/>
-      <c r="B7" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="74" t="s">
+    <row r="17" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B17" s="65"/>
+      <c r="C17" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="E17" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="66">
-        <v>0.06</v>
-      </c>
-      <c r="E7" s="23" t="s">
-        <v>100</v>
-      </c>
-      <c r="H7" s="51"/>
+      <c r="F17" s="66">
+        <v>0.37</v>
+      </c>
+      <c r="G17" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="J17" s="51"/>
     </row>
-    <row r="8" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A8" s="65"/>
-      <c r="B8" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" s="74" t="s">
+    <row r="18" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B18" s="65"/>
+      <c r="C18" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="E18" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="66">
-        <v>0.4</v>
-      </c>
-      <c r="E8" s="23" t="s">
-        <v>101</v>
-      </c>
-      <c r="H8" s="51"/>
+      <c r="F18" s="66">
+        <v>-0.32</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>108</v>
+      </c>
+      <c r="J18" s="51"/>
     </row>
-    <row r="9" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A9" s="65"/>
-      <c r="B9" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="74" t="s">
+    <row r="19" spans="2:10" ht="17" x14ac:dyDescent="0.2">
+      <c r="B19" s="65"/>
+      <c r="C19" s="95" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="73" t="s">
+        <v>120</v>
+      </c>
+      <c r="E19" s="74" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="66">
-        <v>-0.53</v>
-      </c>
-      <c r="E9" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="H9" s="51"/>
+      <c r="F19" s="66">
+        <v>-0.19</v>
+      </c>
+      <c r="G19" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" s="51"/>
     </row>
-    <row r="10" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="65"/>
-      <c r="B10" s="73" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="74" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="66">
-        <v>-0.4</v>
-      </c>
-      <c r="E10" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="H10" s="51"/>
-    </row>
-    <row r="11" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A11" s="76"/>
-      <c r="B11" s="77" t="s">
-        <v>91</v>
-      </c>
-      <c r="C11" s="78" t="s">
-        <v>90</v>
-      </c>
-      <c r="D11" s="23" t="s">
-        <v>110</v>
-      </c>
-      <c r="E11" s="23" t="s">
-        <v>111</v>
-      </c>
-      <c r="H11" s="51"/>
-    </row>
-    <row r="12" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A12" s="65"/>
-      <c r="B12" s="73" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="74" t="s">
-        <v>32</v>
-      </c>
-      <c r="D12" s="66">
-        <v>-0.24</v>
-      </c>
-      <c r="E12" s="79" t="s">
-        <v>104</v>
-      </c>
-      <c r="H12" s="51"/>
-    </row>
-    <row r="13" spans="1:8" ht="73" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="65"/>
-      <c r="B13" s="73" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="74" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="66">
-        <v>-5.83</v>
-      </c>
-      <c r="E13" s="79" t="s">
-        <v>105</v>
-      </c>
-      <c r="H13" s="51"/>
-    </row>
-    <row r="14" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="A14" s="65"/>
-      <c r="B14" s="73" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="23" t="s">
-        <v>96</v>
-      </c>
-      <c r="E14" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="H14" s="51"/>
-    </row>
-    <row r="15" spans="1:8" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="65"/>
-      <c r="B15" s="73" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="D15" s="66">
-        <v>0.36</v>
-      </c>
-      <c r="E15" s="79" t="s">
-        <v>106</v>
-      </c>
-      <c r="H15" s="51"/>
-    </row>
-    <row r="16" spans="1:8" ht="34" x14ac:dyDescent="0.2">
-      <c r="A16" s="80"/>
-      <c r="B16" s="73" t="s">
-        <v>83</v>
-      </c>
-      <c r="C16" s="74" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="66">
-        <v>17.28</v>
-      </c>
-      <c r="E16" s="79" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="51"/>
-    </row>
-    <row r="17" spans="1:8" ht="35" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="71"/>
-      <c r="B17" s="53" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="82" t="s">
-        <v>86</v>
-      </c>
-      <c r="D17" s="67">
-        <v>18.96</v>
-      </c>
-      <c r="E17" s="81" t="s">
-        <v>108</v>
-      </c>
-      <c r="H17" s="51"/>
-    </row>
-    <row r="21" spans="1:8" ht="68" x14ac:dyDescent="0.2">
-      <c r="B21" s="27" t="s">
-        <v>60</v>
+    <row r="23" spans="2:10" ht="68" x14ac:dyDescent="0.2">
+      <c r="D23" s="27" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A12:B12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -5714,23 +5899,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17" x14ac:dyDescent="0.2">
@@ -5751,7 +5936,7 @@
     </row>
     <row r="6" spans="1:2" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>18</v>
@@ -5782,7 +5967,7 @@
     <row r="12" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
@@ -5819,13 +6004,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="54" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B1" s="55" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C1" s="62" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D1" s="56" t="s">
         <v>1</v>
@@ -5833,80 +6018,80 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="57" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C2" s="63">
         <v>4.1100000000000003</v>
       </c>
       <c r="D2" s="58" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="57"/>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="63">
         <v>4.12</v>
       </c>
       <c r="D3" s="58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="57" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C4" s="63">
         <v>4.13</v>
       </c>
       <c r="D4" s="58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="57" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="63">
         <v>4.1399999999999997</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="59" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B6" s="60" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C6" s="64">
         <v>4.1500000000000004</v>
       </c>
       <c r="D6" s="61" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>